<commit_message>
to test FI_T behavior when no process parameters defined.
</commit_message>
<xml_diff>
--- a/VT_REG2_TRA_V12.xlsx
+++ b/VT_REG2_TRA_V12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F85117-2115-4CBE-BFA8-FF45E261CE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953959BF-F346-4361-A37B-6D15DB1E97C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2145" windowWidth="21600" windowHeight="12683" tabRatio="901" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="901" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EB2" sheetId="133" r:id="rId1"/>
@@ -1534,7 +1534,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="208">
   <si>
     <t>CommName</t>
   </si>
@@ -2125,6 +2125,39 @@
   </si>
   <si>
     <t>~PRCCOMEMI</t>
+  </si>
+  <si>
+    <t>TRAGAS</t>
+  </si>
+  <si>
+    <t>COM_PROJ</t>
+  </si>
+  <si>
+    <t>TCAR_TEST-bad</t>
+  </si>
+  <si>
+    <t>TCAR_TEST-good</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>TRABIO</t>
+  </si>
+  <si>
+    <t>TRAELC</t>
+  </si>
+  <si>
+    <t>DTCAR_test</t>
+  </si>
+  <si>
+    <t>to test FI_T behavior</t>
+  </si>
+  <si>
+    <t>Test FI_T issue - does not work</t>
+  </si>
+  <si>
+    <t>Test FI_T issue - works</t>
   </si>
 </sst>
 </file>
@@ -6578,10 +6611,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7819,6 +7852,215 @@
     <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
     </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>204</v>
+      </c>
+      <c r="E35" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="O38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>198</v>
+      </c>
+      <c r="L39"/>
+      <c r="O39" t="s">
+        <v>11</v>
+      </c>
+      <c r="P39" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>1</v>
+      </c>
+      <c r="R39" t="s">
+        <v>2</v>
+      </c>
+      <c r="S39" t="s">
+        <v>16</v>
+      </c>
+      <c r="T39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" t="s">
+        <v>204</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="L40"/>
+      <c r="O40" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q40" t="str">
+        <f>B40</f>
+        <v>TCAR_TEST-bad</v>
+      </c>
+      <c r="R40" t="s">
+        <v>206</v>
+      </c>
+      <c r="S40" t="s">
+        <v>180</v>
+      </c>
+      <c r="T40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="O44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>198</v>
+      </c>
+      <c r="F45" t="s">
+        <v>201</v>
+      </c>
+      <c r="L45"/>
+      <c r="O45" t="s">
+        <v>11</v>
+      </c>
+      <c r="P45" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>2</v>
+      </c>
+      <c r="S45" t="s">
+        <v>16</v>
+      </c>
+      <c r="T45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" t="s">
+        <v>204</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="L46"/>
+      <c r="O46" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q46" t="str">
+        <f>B46</f>
+        <v>TCAR_TEST-good</v>
+      </c>
+      <c r="R46" t="s">
+        <v>207</v>
+      </c>
+      <c r="S46" t="s">
+        <v>180</v>
+      </c>
+      <c r="T46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7830,7 +8072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>